<commit_message>
Elegir carpeta y Sharp
</commit_message>
<xml_diff>
--- a/Materiales.xlsx
+++ b/Materiales.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Desktop\Acoustica 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Desktop\Acoustica_2\GUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Material</t>
   </si>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t>Densidad</t>
-  </si>
-  <si>
-    <t>Usuario</t>
   </si>
 </sst>
 </file>
@@ -493,7 +490,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,9 +805,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="9" t="s">
-        <v>20</v>
-      </c>
+      <c r="B16" s="9"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
     </row>

</xml_diff>